<commit_message>
lineup catalog for online
</commit_message>
<xml_diff>
--- a/lineups/HELIO4CAST_multipoint_v10.xlsx
+++ b/lineups/HELIO4CAST_multipoint_v10.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ICMECATv2.0" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HELIO4CAST multipoint ICME catalog v1.0" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -59,12 +56,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -378,7 +374,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>start time</t>
+          <t>event_start_time</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -388,32 +384,32 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>R [AU]</t>
+          <t>sc_heliodistance</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>sc long. [HEEQ]</t>
+          <t>sc_heeq_lon</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>CME long. [HEEQ]</t>
+          <t>cme_heeq_lon</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>speed [km/s]</t>
+          <t>speed</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Bt max [nT]</t>
+          <t>mo_bmax</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Bz min [nT]</t>
+          <t>mo_bzmin</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -429,8 +425,10 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>43936.86736111111</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2020-04-15T20:49Z</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -472,8 +470,10 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>43940.2125</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2020-04-19T05:06Z</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -515,8 +515,10 @@
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>43941.06527777778</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2020-04-20T01:34Z</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -556,8 +558,10 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>43941.13125</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2020-04-20T03:09Z</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -599,8 +603,10 @@
       <c r="B6" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>43977.06180555555</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2020-05-26T01:29Z</t>
+        </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -642,8 +648,10 @@
       <c r="B7" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>43979.53125</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2020-05-28T12:45Z</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -685,8 +693,10 @@
       <c r="B8" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>43980.88888888889</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2020-05-29T21:20Z</t>
+        </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -726,8 +736,10 @@
       <c r="B9" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>43980.64375</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2020-05-29T15:27Z</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -769,8 +781,10 @@
       <c r="B10" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>43978.20069444444</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2020-05-27T04:49Z</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -812,8 +826,10 @@
       <c r="B11" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>43985.32916666667</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2020-06-03T07:54Z</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -853,8 +869,10 @@
       <c r="B12" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>44005.03402777778</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2020-06-23T00:49Z</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -896,8 +914,10 @@
       <c r="B13" t="n">
         <v>4</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>44007.66597222222</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2020-06-25T15:59Z</t>
+        </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -937,8 +957,10 @@
       <c r="B14" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>44011.40555555555</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2020-06-29T09:44Z</t>
+        </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -980,8 +1002,10 @@
       <c r="B15" t="n">
         <v>4</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>44013.02777777778</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2020-07-01T00:40Z</t>
+        </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1021,8 +1045,10 @@
       <c r="B16" t="n">
         <v>5</v>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>44018.25625</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2020-07-06T06:09Z</t>
+        </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1064,8 +1090,10 @@
       <c r="B17" t="n">
         <v>5</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>44021.59513888889</v>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2020-07-09T14:17Z</t>
+        </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1105,8 +1133,10 @@
       <c r="B18" t="n">
         <v>6</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>44021.36736111111</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2020-07-09T08:49Z</t>
+        </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1148,8 +1178,10 @@
       <c r="B19" t="n">
         <v>6</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>44025.84583333333</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2020-07-13T20:18Z</t>
+        </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1189,8 +1221,10 @@
       <c r="B20" t="n">
         <v>7</v>
       </c>
-      <c r="C20" s="2" t="n">
-        <v>44059.58958333333</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2020-08-16T14:09Z</t>
+        </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1232,8 +1266,10 @@
       <c r="B21" t="n">
         <v>7</v>
       </c>
-      <c r="C21" s="2" t="n">
-        <v>44062.88263888889</v>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2020-08-19T21:11Z</t>
+        </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1275,8 +1311,10 @@
       <c r="B22" t="n">
         <v>8</v>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>44082.70069444444</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2020-09-08T16:49Z</t>
+        </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1318,8 +1356,10 @@
       <c r="B23" t="n">
         <v>8</v>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>44086.43263888889</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2020-09-12T10:23Z</t>
+        </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1359,8 +1399,10 @@
       <c r="B24" t="n">
         <v>9</v>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>44104.78402777778</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2020-09-30T18:49Z</t>
+        </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1402,8 +1444,10 @@
       <c r="B25" t="n">
         <v>9</v>
       </c>
-      <c r="C25" s="2" t="n">
-        <v>44109.28611111111</v>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2020-10-05T06:52Z</t>
+        </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1443,8 +1487,10 @@
       <c r="B26" t="n">
         <v>10</v>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>44110.64513888889</v>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2020-10-06T15:29Z</t>
+        </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1486,8 +1532,10 @@
       <c r="B27" t="n">
         <v>10</v>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>44112.43541666667</v>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2020-10-08T10:27Z</t>
+        </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1529,8 +1577,10 @@
       <c r="B28" t="n">
         <v>10</v>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>44114.17152777778</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2020-10-10T04:07Z</t>
+        </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1572,8 +1622,10 @@
       <c r="B29" t="n">
         <v>11</v>
       </c>
-      <c r="C29" s="2" t="n">
-        <v>44130.81180555555</v>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2020-10-26T19:29Z</t>
+        </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1615,8 +1667,10 @@
       <c r="B30" t="n">
         <v>11</v>
       </c>
-      <c r="C30" s="2" t="n">
-        <v>44136.49583333333</v>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2020-11-01T11:54Z</t>
+        </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1656,8 +1710,10 @@
       <c r="B31" t="n">
         <v>12</v>
       </c>
-      <c r="C31" s="2" t="n">
-        <v>44166.09861111111</v>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2020-12-01T02:22Z</t>
+        </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1699,8 +1755,10 @@
       <c r="B32" t="n">
         <v>12</v>
       </c>
-      <c r="C32" s="2" t="n">
-        <v>44166.31111111111</v>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2020-12-01T07:28Z</t>
+        </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1742,8 +1800,10 @@
       <c r="B33" t="n">
         <v>13</v>
       </c>
-      <c r="C33" s="2" t="n">
-        <v>44164.67291666667</v>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2020-11-29T16:09Z</t>
+        </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1785,8 +1845,10 @@
       <c r="B34" t="n">
         <v>13</v>
       </c>
-      <c r="C34" s="2" t="n">
-        <v>44166.45069444444</v>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2020-12-01T10:49Z</t>
+        </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1828,8 +1890,10 @@
       <c r="B35" t="n">
         <v>13</v>
       </c>
-      <c r="C35" s="2" t="n">
-        <v>44168.75277777778</v>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2020-12-03T18:04Z</t>
+        </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1871,8 +1935,10 @@
       <c r="B36" t="n">
         <v>14</v>
       </c>
-      <c r="C36" s="2" t="n">
-        <v>44238.06180555555</v>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2021-02-11T01:29Z</t>
+        </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1914,8 +1980,10 @@
       <c r="B37" t="n">
         <v>14</v>
       </c>
-      <c r="C37" s="2" t="n">
-        <v>44242.79027777778</v>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2021-02-15T18:58Z</t>
+        </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1955,8 +2023,10 @@
       <c r="B38" t="n">
         <v>15</v>
       </c>
-      <c r="C38" s="2" t="n">
-        <v>44247.7</v>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2021-02-20T16:48Z</t>
+        </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1998,8 +2068,10 @@
       <c r="B39" t="n">
         <v>15</v>
       </c>
-      <c r="C39" s="2" t="n">
-        <v>44250.44027777778</v>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2021-02-23T10:34Z</t>
+        </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -2041,8 +2113,10 @@
       <c r="B40" t="n">
         <v>15</v>
       </c>
-      <c r="C40" s="2" t="n">
-        <v>44251.17222222222</v>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2021-02-24T04:08Z</t>
+        </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -2082,8 +2156,10 @@
       <c r="B41" t="n">
         <v>16</v>
       </c>
-      <c r="C41" s="2" t="n">
-        <v>44277.36666666667</v>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2021-03-22T08:48Z</t>
+        </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -2125,8 +2201,10 @@
       <c r="B42" t="n">
         <v>16</v>
       </c>
-      <c r="C42" s="2" t="n">
-        <v>44281.75</v>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2021-03-26T18:00Z</t>
+        </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -2166,8 +2244,10 @@
       <c r="B43" t="n">
         <v>17</v>
       </c>
-      <c r="C43" s="2" t="n">
-        <v>44286.00555555556</v>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2021-03-31T00:08Z</t>
+        </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -2209,8 +2289,10 @@
       <c r="B44" t="n">
         <v>17</v>
       </c>
-      <c r="C44" s="2" t="n">
-        <v>44290.91111111111</v>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2021-04-04T21:52Z</t>
+        </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -2250,8 +2332,10 @@
       <c r="B45" t="n">
         <v>17</v>
       </c>
-      <c r="C45" s="2" t="n">
-        <v>44292.06041666667</v>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2021-04-06T01:27Z</t>
+        </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -2293,8 +2377,10 @@
       <c r="B46" t="n">
         <v>18</v>
       </c>
-      <c r="C46" s="2" t="n">
-        <v>44296.75555555556</v>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2021-04-10T18:08Z</t>
+        </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -2336,8 +2422,10 @@
       <c r="B47" t="n">
         <v>18</v>
       </c>
-      <c r="C47" s="2" t="n">
-        <v>44301.13611111111</v>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2021-04-15T03:16Z</t>
+        </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
added low_latency in solo, lineup cat
</commit_message>
<xml_diff>
--- a/lineups/HELIO4CAST_multipoint_v10.xlsx
+++ b/lineups/HELIO4CAST_multipoint_v10.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2370,94 +2370,6 @@
         </is>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="n">
-        <v>18</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>2021-04-10T18:08Z</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>HIA</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>0.967</v>
-      </c>
-      <c r="F46" t="n">
-        <v>-54.1</v>
-      </c>
-      <c r="G46" t="n">
-        <v>14</v>
-      </c>
-      <c r="H46" t="n">
-        <v>412</v>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>HCME_A__20210410_01</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="n">
-        <v>18</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>2021-04-15T03:16Z</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Wind</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>0.995</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H47" t="n">
-        <v>382</v>
-      </c>
-      <c r="I47" t="n">
-        <v>10.6</v>
-      </c>
-      <c r="J47" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>ICME_Wind_MOESTL_20210415_01</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
icmecat and lineupcat update
</commit_message>
<xml_diff>
--- a/lineups/HELIO4CAST_multipoint_v10.xlsx
+++ b/lineups/HELIO4CAST_multipoint_v10.xlsx
@@ -916,7 +916,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2020-06-25T15:59Z</t>
+          <t>2020-06-25T11:39Z</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -984,10 +984,10 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>8.6</v>
+        <v>11.4</v>
       </c>
       <c r="J14" t="n">
-        <v>-3.7</v>
+        <v>-7.8</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2020-07-01T00:40Z</t>
+          <t>2020-06-30T01:12Z</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="I15" t="n">
         <v>6.4</v>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>ICME_Wind_MOESTL_20200701_01</t>
+          <t>ICME_Wind_MOESTL_20200630_01</t>
         </is>
       </c>
     </row>

</xml_diff>